<commit_message>
correction to L05/06, and new lectures
</commit_message>
<xml_diff>
--- a/Misc/15CS43-DAA-Lecture-Plan.xlsx
+++ b/Misc/15CS43-DAA-Lecture-Plan.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="17140" windowHeight="17260" activeTab="1"/>
+    <workbookView xWindow="10500" yWindow="640" windowWidth="17140" windowHeight="17260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="COs" sheetId="2" r:id="rId1"/>
     <sheet name="Plan" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="118">
   <si>
     <t>Date</t>
   </si>
@@ -343,13 +344,95 @@
   <si>
     <t>Divide and Conquer: General method, Binary search. Recurrence equation  (T2: 3.1,3.3)</t>
   </si>
+  <si>
+    <t>L01_02</t>
+  </si>
+  <si>
+    <t>L03</t>
+  </si>
+  <si>
+    <t>L04</t>
+  </si>
+  <si>
+    <t>L05_06</t>
+  </si>
+  <si>
+    <t>L07_08</t>
+  </si>
+  <si>
+    <t>L09_10</t>
+  </si>
+  <si>
+    <t>L11_12</t>
+  </si>
+  <si>
+    <t>L13_14</t>
+  </si>
+  <si>
+    <t>L15_16</t>
+  </si>
+  <si>
+    <t>L17_18</t>
+  </si>
+  <si>
+    <t>L19_20</t>
+  </si>
+  <si>
+    <t>L21_22</t>
+  </si>
+  <si>
+    <t>L23_24</t>
+  </si>
+  <si>
+    <t>L25_26</t>
+  </si>
+  <si>
+    <t>L27_28</t>
+  </si>
+  <si>
+    <t>L29_30</t>
+  </si>
+  <si>
+    <t>L31_32</t>
+  </si>
+  <si>
+    <t>L33_34</t>
+  </si>
+  <si>
+    <t>L35_36</t>
+  </si>
+  <si>
+    <t>L37_38</t>
+  </si>
+  <si>
+    <t>L39_40</t>
+  </si>
+  <si>
+    <t>L41_42</t>
+  </si>
+  <si>
+    <t>L43_44</t>
+  </si>
+  <si>
+    <t>L45_46</t>
+  </si>
+  <si>
+    <t>L47_48</t>
+  </si>
+  <si>
+    <t>L49_50</t>
+  </si>
+  <si>
+    <t>L51_52</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="\L00"/>
+    <numFmt numFmtId="166" formatCode="[$-14009]dd\-mm\-yy;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -513,7 +596,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="287">
+  <cellStyleXfs count="295">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -801,8 +884,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -849,11 +940,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -861,11 +949,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="287">
+  <cellStyles count="295">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1009,6 +1104,10 @@
     <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1152,6 +1251,10 @@
     <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1187,7 +1290,7 @@
         <xdr:cNvPr id="2" name="Picture 1" descr="page5image5008736">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{408C81D5-4E96-9C45-AEFF-C45C0728AE98}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{408C81D5-4E96-9C45-AEFF-C45C0728AE98}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1248,7 +1351,7 @@
         <xdr:cNvPr id="3" name="Picture 2" descr="page6image5061712">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{13AD06D1-DC2F-7D44-85E0-679C31939DB7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13AD06D1-DC2F-7D44-85E0-679C31939DB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1583,7 +1686,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1657,10 +1760,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F52"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1670,767 +1773,769 @@
     <col min="3" max="3" width="2.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="76.33203125" style="5" customWidth="1"/>
     <col min="5" max="5" width="6.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" style="24" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" style="20" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
-      <c r="A2" s="7" t="s">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="7" spans="1:6" ht="25.5" customHeight="1"/>
+    <row r="11" spans="1:6">
+      <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="9">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="13">
-        <v>2</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="21"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="13">
-        <v>3</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="21"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="13">
-        <v>4</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="13">
-        <v>5</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="13">
-        <v>6</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="21"/>
-    </row>
-    <row r="9" spans="1:6" ht="30">
-      <c r="A9" s="13">
-        <v>7</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="21"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="16">
-        <v>8</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="21"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="9">
-        <v>9</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="9">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="10"/>
-      <c r="D12" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="21"/>
+      <c r="D12" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="13">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="14"/>
-      <c r="D13" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="21"/>
+      <c r="D13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="22"/>
+      <c r="F13" s="24"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="13">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="21"/>
+        <v>42</v>
+      </c>
+      <c r="E14" s="22"/>
+      <c r="F14" s="24"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="13">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>34</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="24"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="13">
+        <v>5</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>14</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>15</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="21"/>
+        <v>89</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="13">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="14"/>
-      <c r="D17" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="23"/>
-      <c r="F17" s="21"/>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="D17" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="22"/>
+      <c r="F17" s="24"/>
+    </row>
+    <row r="18" spans="1:6" ht="30">
       <c r="A18" s="13">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="21"/>
+        <v>43</v>
+      </c>
+      <c r="E18" s="22"/>
+      <c r="F18" s="24"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="13">
-        <v>17</v>
-      </c>
-      <c r="B19" s="13" t="s">
+      <c r="A19" s="16">
+        <v>8</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="22"/>
+      <c r="F19" s="24"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="9">
+        <v>9</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="9">
+        <v>10</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="13">
-        <v>18</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="21"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="13">
-        <v>19</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="23"/>
-      <c r="F21" s="21"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="22"/>
+      <c r="F21" s="24"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="13">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C22" s="14"/>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="22"/>
+      <c r="F22" s="24"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="13">
+        <v>12</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="22"/>
+      <c r="F23" s="24"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="13">
+        <v>13</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="13">
+        <v>14</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="22"/>
+      <c r="F25" s="24"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="13">
+        <v>15</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="22"/>
+      <c r="F26" s="24"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="13">
+        <v>16</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="22"/>
+      <c r="F27" s="24"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="13">
+        <v>17</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="13">
+        <v>18</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="22"/>
+      <c r="F29" s="24"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="13">
+        <v>19</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="22"/>
+      <c r="F30" s="24"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="13">
+        <v>20</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="23"/>
-      <c r="F22" s="21"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="7">
+      <c r="E31" s="22"/>
+      <c r="F31" s="24"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="7">
         <v>21</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B32" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E32" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F32" s="23" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="7">
-        <v>22</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" s="23"/>
-      <c r="F24" s="21"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="7">
-        <v>23</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="23"/>
-      <c r="F25" s="21"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="7">
-        <v>24</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="23"/>
-      <c r="F26" s="21"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="7">
-        <v>25</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="7">
-        <v>26</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="23"/>
-      <c r="F28" s="21"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="7">
-        <v>27</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E29" s="23"/>
-      <c r="F29" s="21"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="7">
-        <v>28</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" s="23"/>
-      <c r="F30" s="21"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="7">
-        <v>29</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="9">
-        <v>30</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="21"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="7">
-        <v>31</v>
-      </c>
-      <c r="B33" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E33" s="23"/>
-      <c r="F33" s="21"/>
+      <c r="D33" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="22"/>
+      <c r="F33" s="24"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="7">
-        <v>32</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E34" s="23"/>
-      <c r="F34" s="21"/>
+        <v>70</v>
+      </c>
+      <c r="E34" s="22"/>
+      <c r="F34" s="24"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="7">
-        <v>33</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>17</v>
+        <v>24</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>36</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="E35" s="22"/>
+      <c r="F35" s="24"/>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="7">
-        <v>34</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="21"/>
+        <v>72</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="7">
-        <v>35</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>17</v>
+        <v>26</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="21"/>
+        <v>73</v>
+      </c>
+      <c r="E37" s="22"/>
+      <c r="F37" s="24"/>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="7">
-        <v>36</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E38" s="23"/>
-      <c r="F38" s="21"/>
+        <v>27</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" s="22"/>
+      <c r="F38" s="24"/>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="7">
-        <v>37</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>60</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="22"/>
+      <c r="F39" s="24"/>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="7">
-        <v>38</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E40" s="23"/>
-      <c r="F40" s="21"/>
+        <v>75</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="7">
-        <v>39</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="21"/>
+      <c r="A41" s="9">
+        <v>30</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="10"/>
+      <c r="D41" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="22"/>
+      <c r="F41" s="24"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="9">
-        <v>40</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E42" s="23"/>
-      <c r="F42" s="21"/>
+      <c r="A42" s="7">
+        <v>31</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E42" s="22"/>
+      <c r="F42" s="24"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="7">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E43" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>38</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E43" s="22"/>
+      <c r="F43" s="24"/>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="7">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E44" s="23"/>
-      <c r="F44" s="21"/>
+        <v>78</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="7">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E45" s="23"/>
-      <c r="F45" s="21"/>
+        <v>53</v>
+      </c>
+      <c r="E45" s="22"/>
+      <c r="F45" s="24"/>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="7">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E46" s="23"/>
-      <c r="F46" s="21"/>
+        <v>79</v>
+      </c>
+      <c r="E46" s="22"/>
+      <c r="F46" s="24"/>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="7">
-        <v>45</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E47" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F47" s="20" t="s">
-        <v>39</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E47" s="22"/>
+      <c r="F47" s="24"/>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="7">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E48" s="23"/>
-      <c r="F48" s="21"/>
-    </row>
-    <row r="49" spans="1:6" ht="31">
+        <v>80</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="7">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E49" s="23"/>
-      <c r="F49" s="21"/>
+        <v>81</v>
+      </c>
+      <c r="E49" s="22"/>
+      <c r="F49" s="24"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="9">
-        <v>48</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C50" s="10"/>
-      <c r="D50" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E50" s="23"/>
-      <c r="F50" s="21"/>
+      <c r="A50" s="7">
+        <v>39</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E50" s="22"/>
+      <c r="F50" s="24"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="7">
-        <v>49</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="A51" s="9">
+        <v>40</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="10"/>
+      <c r="D51" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E51" s="22"/>
+      <c r="F51" s="24"/>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="7">
+        <v>41</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="7">
+        <v>42</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E53" s="22"/>
+      <c r="F53" s="24"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="7">
+        <v>43</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E54" s="22"/>
+      <c r="F54" s="24"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="7">
+        <v>44</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E55" s="22"/>
+      <c r="F55" s="24"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="7">
+        <v>45</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E56" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="7">
+        <v>46</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" s="22"/>
+      <c r="F57" s="24"/>
+    </row>
+    <row r="58" spans="1:6" ht="31">
+      <c r="A58" s="7">
+        <v>47</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E58" s="22"/>
+      <c r="F58" s="24"/>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="9">
+        <v>48</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" s="10"/>
+      <c r="D59" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E59" s="22"/>
+      <c r="F59" s="24"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="7">
+        <v>49</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="7">
         <v>50</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B61" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D61" s="5" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="E47:E50"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="E43:E46"/>
-    <mergeCell ref="F47:F50"/>
-    <mergeCell ref="F3:F6"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="F31:F34"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="F39:F42"/>
-    <mergeCell ref="F43:F46"/>
+    <mergeCell ref="F56:F59"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="F32:F35"/>
+    <mergeCell ref="F36:F39"/>
+    <mergeCell ref="F40:F43"/>
+    <mergeCell ref="F44:F47"/>
+    <mergeCell ref="F48:F51"/>
+    <mergeCell ref="F52:F55"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="E44:E47"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="E52:E55"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
@@ -2441,4 +2546,399 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:D39"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="25"/>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4">
+      <c r="B3" s="25">
+        <v>43503</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="25">
+        <v>43509</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="25">
+        <v>43510</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="25">
+        <v>43515</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="25">
+        <v>43517</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="25">
+        <v>43519</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="25">
+        <v>43522</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="25">
+        <v>43524</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="25">
+        <v>43529</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="25">
+        <v>43531</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="25">
+        <v>43538</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="25">
+        <v>43543</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="25">
+        <v>43545</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="25">
+        <v>43550</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="25">
+        <v>43552</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="25">
+        <v>43557</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="25">
+        <v>43559</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="25">
+        <v>43564</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="25">
+        <v>43566</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="25">
+        <v>43568</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="25">
+        <v>43571</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="25">
+        <v>43578</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="25">
+        <v>43580</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="25">
+        <v>43585</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="25">
+        <v>43587</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="25">
+        <v>43594</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="25">
+        <v>43599</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="25">
+        <v>43601</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="25">
+        <v>43606</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="25">
+        <v>43608</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" s="25">
+        <v>43610</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" s="25">
+        <v>43613</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="25">
+        <v>43615</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" s="25">
+        <v>43620</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="25">
+        <v>43622</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="C39">
+        <f>SUM(C3:C37)</f>
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B3:D122">
+    <sortCondition ref="D3:D122"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>